<commit_message>
Three sticky notes to go
</commit_message>
<xml_diff>
--- a/Relevant Documents/Self-emails.xlsx
+++ b/Relevant Documents/Self-emails.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,6 @@
     <definedName name="_xlchart.0" hidden="1">Sheet1!$E$2:$F$7</definedName>
     <definedName name="_xlchart.1" hidden="1">Sheet1!$G$1</definedName>
     <definedName name="_xlchart.2" hidden="1">Sheet1!$G$2:$G$7</definedName>
-    <definedName name="_xlchart.3" hidden="1">Sheet1!$E$2:$F$7</definedName>
-    <definedName name="_xlchart.4" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.5" hidden="1">Sheet1!$G$2:$G$7</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1965,7 +1962,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,6 +2189,10 @@
       <c r="C8">
         <v>29</v>
       </c>
+      <c r="N8">
+        <f>SUM(N6,N7)</f>
+        <v>1198</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2202,6 +2203,10 @@
       </c>
       <c r="C9">
         <v>6</v>
+      </c>
+      <c r="N9">
+        <f>SUM(N2:N7)</f>
+        <v>1950</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>